<commit_message>
clean up; getting close to Wouter's results.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
+++ b/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\EU_TIMES_Veda2p0\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FE40A-153D-4D2C-A1E3-B2C09CCAFC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC6C77F-B72A-48CD-994C-A6BFAA6C212B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="570" windowWidth="25080" windowHeight="15030" tabRatio="909" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="750" windowWidth="21600" windowHeight="11385" tabRatio="909" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill Data" sheetId="25" r:id="rId1"/>

</xml_diff>

<commit_message>
updates from Wouter 30Jan21
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
+++ b/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC6C77F-B72A-48CD-994C-A6BFAA6C212B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9C5D24-8BCB-4E00-BA52-C68D519D887E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="750" windowWidth="21600" windowHeight="11385" tabRatio="909" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="3390" windowWidth="15825" windowHeight="12210" tabRatio="909" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill Data" sheetId="25" r:id="rId1"/>

</xml_diff>